<commit_message>
Sol Graf. CN 06 04 REC130 (nueva)
Sol Graf. CN 06 04 REC130 (nueva)
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion04/SolicitudGrafic_CN_06_04_CO_REC130.xlsx
+++ b/fuentes/contenidos/grado06/guion04/SolicitudGrafic_CN_06_04_CO_REC130.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado06\guion04\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Dropbox\Editorial planeta\1. Autor\Escaletas\CN_06_04_CO\Recursos DM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="201">
   <si>
     <t>Fecha:</t>
   </si>
@@ -602,19 +602,34 @@
     <t>Ilustración</t>
   </si>
   <si>
-    <t>Iluminar lo relacionado a difusión facilitada encerrado en rojo en la imagen y las palabras en común.</t>
-  </si>
-  <si>
-    <t>Iluminar lo relacionado con el transporte activo encerrado en rojo y las palabras en común.</t>
-  </si>
-  <si>
-    <t>Está imagen ya está en el cuaderno de estudio, utilizar la misma imagen. IMG08    (Tener en cuenta de rellenar bien, en color verde, la molécula que está al lado de las palabras 1. Difusión simple.  Y realizar el cambio de las palabras Bomba de proteína por  Proteína de membrana)</t>
-  </si>
-  <si>
-    <t>Iluminar lo relacionado con la difusión simple.  Por lo tanto iluminar lo siguiente:          Las palabras: Transporte pasivo     1. Disusión simple       Moléculas transportadas                                                                                      En la imagen se muestra con encerramiento en color rojo lo que se debe ilumnar.                                                                                   Tanto en esta imagen como en las dos siguientes (img03 e Img04) iluminar las palabras en común con las respetivas lineas de señalaiento:   Bicapa fosfolipídica, Fluido extracelular,  Fuera de la célula, Membrana celular, Dentro de la célula, Alta conecntración de sustancias, Baja concentración de sustancias, Citoplasma</t>
-  </si>
-  <si>
     <t>Transporte en membrana celular</t>
+  </si>
+  <si>
+    <t>Eliminar las sigueintes palabras                                            "Cell memebrane",  "Glycoprotein", "Oligosaccharide", "Glycolipid".   "ionic channel".                                                                             Cambiar las palabras en inglés a español así:                                           Protein complex:  Proteína canal                                       Alpha helix proteín:  Proteína integral                                 Integral proteín: Proteína integral                                             Señalar la bicapa fosfolípidica como esta en la imagen.</t>
+  </si>
+  <si>
+    <t>https://commons.wikimedia.org/wiki/File:Scheme_simple_diffusion_in_cell_membrane-es.svg</t>
+  </si>
+  <si>
+    <t>Transporte pasivo: difusción simple</t>
+  </si>
+  <si>
+    <t>Borrar la palabra tiempo y la  línea azul que está justo al lado.   Cambiar la palabra lípida por lipídica.     En la parte superior del lado izquierdo de la imagen incluir:  Alta concentración de sustancias   y en la parte inferior   Baja concentración de sustancias, como se muestra en la imagen.</t>
+  </si>
+  <si>
+    <t>https://commons.wikimedia.org/wiki/File:Scheme_facilitated_diffusion_in_cell_membrane-es.svg?uselang=es</t>
+  </si>
+  <si>
+    <t>Transporte pasivo: difusión facilitada</t>
+  </si>
+  <si>
+    <t>Sin cambios</t>
+  </si>
+  <si>
+    <t>https://commons.wikimedia.org/wiki/File:Scheme_sodium-potassium_pump-gl.svg</t>
+  </si>
+  <si>
+    <t>Transporte activo (bomba de sodio-potasio)</t>
   </si>
 </sst>
 </file>
@@ -1780,19 +1795,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>508017</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>40822</xdr:rowOff>
+      <xdr:colOff>68035</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>81642</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>2703641</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>1912158</xdr:rowOff>
+      <xdr:colOff>2993571</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1885842</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Imagen 5"/>
+        <xdr:cNvPr id="5" name="Imagen 4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1805,8 +1820,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16877410" y="3360965"/>
-          <a:ext cx="2195624" cy="1871336"/>
+          <a:off x="16437428" y="2204356"/>
+          <a:ext cx="2925536" cy="1804200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1818,19 +1833,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>272142</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>68659</xdr:rowOff>
+      <xdr:colOff>81643</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>244928</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>2956398</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>2394856</xdr:rowOff>
+      <xdr:colOff>3052918</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>2258786</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Imagen 6"/>
+        <xdr:cNvPr id="9" name="Imagen 8"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1843,46 +1858,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16641535" y="7416516"/>
-          <a:ext cx="2684256" cy="2326197"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>299998</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>68035</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>2653393</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>1986062</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Imagen 7"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="16669391" y="10382249"/>
-          <a:ext cx="2353395" cy="1918027"/>
+          <a:off x="16451036" y="5755821"/>
+          <a:ext cx="2971275" cy="2013858"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2609,8 +2586,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C11" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2692,7 +2669,7 @@
       </c>
       <c r="D3" s="88"/>
       <c r="F3" s="80">
-        <v>42307</v>
+        <v>42310</v>
       </c>
       <c r="G3" s="81"/>
       <c r="H3" s="58"/>
@@ -2898,13 +2875,13 @@
         <v>M10B</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="11" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="11" customFormat="1" ht="276" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
       </c>
       <c r="B10" s="62">
-        <v>104022737</v>
+        <v>239311687</v>
       </c>
       <c r="C10" s="20" t="str">
         <f t="shared" ref="C10:C41" si="0">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
@@ -2933,23 +2910,23 @@
         <v/>
       </c>
       <c r="J10" s="63" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="K10" s="64" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O10" s="2" t="str">
         <f>'Definición técnica de imagenes'!A12</f>
         <v>M12D</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="11" customFormat="1" ht="339" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="11" customFormat="1" ht="279" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="str">
         <f t="shared" ref="A11:A18" si="3">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE(LEFT(A10,3),IF(MID(A10,4,2)+1&lt;10,CONCATENATE("0",MID(A10,4,2)+1))),"")</f>
         <v>IMG02</v>
       </c>
-      <c r="B11" s="62">
-        <v>104022737</v>
+      <c r="B11" s="62" t="s">
+        <v>193</v>
       </c>
       <c r="C11" s="20" t="str">
         <f t="shared" si="0"/>
@@ -2978,23 +2955,23 @@
         <v/>
       </c>
       <c r="J11" s="63" t="s">
+        <v>194</v>
+      </c>
+      <c r="K11" s="65" t="s">
         <v>195</v>
-      </c>
-      <c r="K11" s="65" t="s">
-        <v>194</v>
       </c>
       <c r="O11" s="2" t="str">
         <f>'Definición técnica de imagenes'!A13</f>
         <v>M101</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="11" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="11" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG03</v>
       </c>
-      <c r="B12" s="62">
-        <v>104022737</v>
+      <c r="B12" s="62" t="s">
+        <v>196</v>
       </c>
       <c r="C12" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3023,23 +3000,23 @@
         <v/>
       </c>
       <c r="J12" s="63" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="K12" s="64" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="O12" s="2" t="str">
         <f>'Definición técnica de imagenes'!A18</f>
         <v>Diaporama F1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="11" customFormat="1" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="11" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG04</v>
       </c>
-      <c r="B13" s="62">
-        <v>104022737</v>
+      <c r="B13" s="62" t="s">
+        <v>199</v>
       </c>
       <c r="C13" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3068,10 +3045,10 @@
         <v/>
       </c>
       <c r="J13" s="63" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="K13" s="64" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="O13" s="2" t="str">
         <f>'Definición técnica de imagenes'!A19</f>

</xml_diff>